<commit_message>
Full with incorrect label fill
</commit_message>
<xml_diff>
--- a/lab5/Results.xlsx
+++ b/lab5/Results.xlsx
@@ -23,7 +23,7 @@
     <t>Количество баллов</t>
   </si>
   <si>
-    <t>5423</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -93,7 +93,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>374.0</v>
+        <v>352.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mediator method setHealthBar() added
</commit_message>
<xml_diff>
--- a/lab5/Results.xlsx
+++ b/lab5/Results.xlsx
@@ -23,7 +23,7 @@
     <t>Количество баллов</t>
   </si>
   <si>
-    <t/>
+    <t>213123</t>
   </si>
 </sst>
 </file>
@@ -93,7 +93,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>255.0</v>
+        <v>503.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fight class cleaned via Mediator
</commit_message>
<xml_diff>
--- a/lab5/Results.xlsx
+++ b/lab5/Results.xlsx
@@ -23,7 +23,7 @@
     <t>Количество баллов</t>
   </si>
   <si>
-    <t>213123</t>
+    <t/>
   </si>
 </sst>
 </file>
@@ -93,7 +93,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>503.0</v>
+        <v>81.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All GUI elements renamed
</commit_message>
<xml_diff>
--- a/lab5/Results.xlsx
+++ b/lab5/Results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>№</t>
   </si>
@@ -23,7 +23,10 @@
     <t>Количество баллов</t>
   </si>
   <si>
-    <t/>
+    <t>First player</t>
+  </si>
+  <si>
+    <t>Second player</t>
   </si>
 </sst>
 </file>
@@ -68,7 +71,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -93,7 +96,18 @@
         <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>338.0</v>
+        <v>80.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="n">
+        <v>71.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Location moved to Fight class
</commit_message>
<xml_diff>
--- a/lab5/Results.xlsx
+++ b/lab5/Results.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>№</t>
   </si>
@@ -27,6 +27,9 @@
   </si>
   <si>
     <t>Second player</t>
+  </si>
+  <si>
+    <t>лошок</t>
   </si>
 </sst>
 </file>
@@ -71,7 +74,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -110,6 +113,17 @@
         <v>71.0</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>64.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>